<commit_message>
Missing README and the Results in required format
</commit_message>
<xml_diff>
--- a/Results/Final Results/Samples/100Scen/Results_Sample100_05.xlsx
+++ b/Results/Final Results/Samples/100Scen/Results_Sample100_05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\6.Semester\Bachelor-Arbeit\bachelor-thesis\bachelor-thesis\Results\Final Results\Samples\100Scen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9F9A74-603B-42A1-8B02-A9831ADAF500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C49A2BC-B6B8-4095-B996-0D3EBE3B9A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2697,7 +2697,7 @@
         <v>47</v>
       </c>
       <c r="S40" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>